<commit_message>
Design Excel Sheet,Add Function For Add Data
</commit_message>
<xml_diff>
--- a/INVENTORY_MANAGEMENT_SYSTEM/INVENTORY.xlsx
+++ b/INVENTORY_MANAGEMENT_SYSTEM/INVENTORY.xlsx
@@ -13,22 +13,44 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="7" uniqueCount="7">
   <si>
     <t>Created by LibXL trial version 4.2.0. Please buy the LibXL full version for removing this message.</t>
+  </si>
+  <si>
+    <t>INVENTORY MANAGEMENT SYSTEM</t>
+  </si>
+  <si>
+    <t>SR.NO</t>
+  </si>
+  <si>
+    <t>Product Name</t>
+  </si>
+  <si>
+    <t>Product Id</t>
+  </si>
+  <si>
+    <t>Product Price</t>
+  </si>
+  <si>
+    <t>Product Quantity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
     </font>
     <font>
       <color indexed="60"/>
+      <b/>
+    </font>
+    <font>
+      <sz val="14"/>
       <b/>
     </font>
   </fonts>
@@ -72,15 +94,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:IV1"/>
+  <dimension ref="A1:IV2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="10.7109375" customWidth="true"/>
+    <col min="2" max="2" width="50.7109375" customWidth="true"/>
+    <col min="3" max="3" width="15.7109375" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+  </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="true" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -338,6 +367,23 @@
       <c r="IU1" s="1"/>
       <c r="IV1" s="1"/>
     </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:IV1"/>

</xml_diff>